<commit_message>
Finishing: Memastikan semua kode konsisten
</commit_message>
<xml_diff>
--- a/UTS/UTS_POS/public/template_supplier.xlsx
+++ b/UTS/UTS_POS/public/template_supplier.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\Pemrograman_Web_Lanjut\UTS\UTS_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D821373-D5F6-4B00-B948-8AF714152711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E15431-F4BD-4E78-ABF3-4BDC1D8EDF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8148" yWindow="3504" windowWidth="9072" windowHeight="7452" xr2:uid="{7EF0172D-F272-4651-B6D2-7ABEBFC41593}"/>
+    <workbookView xWindow="8328" yWindow="3408" windowWidth="9072" windowHeight="7452" xr2:uid="{7EF0172D-F272-4651-B6D2-7ABEBFC41593}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,31 +45,31 @@
     <t>supplier_alamat</t>
   </si>
   <si>
-    <t>SUP004</t>
-  </si>
-  <si>
     <t>Supplier D</t>
   </si>
   <si>
     <t>Jl. Mawar No. 4</t>
   </si>
   <si>
-    <t>SUP005</t>
-  </si>
-  <si>
     <t>Supplier E</t>
   </si>
   <si>
     <t>Jl. Melati No. 5</t>
   </si>
   <si>
-    <t>SUP006</t>
-  </si>
-  <si>
     <t>Supplier F</t>
   </si>
   <si>
     <t>Jl. Anggrek No. 6</t>
+  </si>
+  <si>
+    <t>asndaSD</t>
+  </si>
+  <si>
+    <t>kjbadJD</t>
+  </si>
+  <si>
+    <t>ASJadbj</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,35 +468,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>